<commit_message>
[feature]: file biểu mẫu mua sắm
</commit_message>
<xml_diff>
--- a/assets/files/bm_mailing_danh_gia.xlsx
+++ b/assets/files/bm_mailing_danh_gia.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\code\vcc\cbms\test\assets\files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tuank\Revotech\VCC\cbms\test\assets\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9EB3F2B1-DA7D-4643-90F9-63C0FFE8C1E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{251A6BCD-471B-4C15-BAB4-C44C4171D67A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-34350" yWindow="5535" windowWidth="28800" windowHeight="15345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="33780" yWindow="450" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Input" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="732" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="796" uniqueCount="52">
   <si>
     <r>
       <t>Mã nhà thầu</t>
@@ -221,10 +221,61 @@
     <t>600.000</t>
   </si>
   <si>
+    <t>Nhà thầu 3</t>
+  </si>
+  <si>
+    <t>01-01-2027</t>
+  </si>
+  <si>
+    <t>7.000.000</t>
+  </si>
+  <si>
+    <t>700.000</t>
+  </si>
+  <si>
     <t>NT001</t>
   </si>
   <si>
     <t>NT002</t>
+  </si>
+  <si>
+    <t>NT003</t>
+  </si>
+  <si>
+    <t>NT004</t>
+  </si>
+  <si>
+    <t>NT005</t>
+  </si>
+  <si>
+    <t>NT006</t>
+  </si>
+  <si>
+    <t>NT007</t>
+  </si>
+  <si>
+    <t>NT008</t>
+  </si>
+  <si>
+    <t>NT009</t>
+  </si>
+  <si>
+    <t>Nhà thầu 4</t>
+  </si>
+  <si>
+    <t>Nhà thầu 5</t>
+  </si>
+  <si>
+    <t>Nhà thầu 6</t>
+  </si>
+  <si>
+    <t>Nhà thầu 7</t>
+  </si>
+  <si>
+    <t>Nhà thầu 8</t>
+  </si>
+  <si>
+    <t>Nhà thầu 9</t>
   </si>
 </sst>
 </file>
@@ -722,10 +773,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J92"/>
+  <dimension ref="A1:J100"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10:XFD10"/>
+      <selection activeCell="A6" sqref="A6:XFD12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -840,7 +891,7 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="12" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="B4" s="12" t="s">
         <v>21</v>
@@ -872,7 +923,7 @@
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="12" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="B5" s="12" t="s">
         <v>27</v>
@@ -901,184 +952,211 @@
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="12" t="s">
-        <v>20</v>
+        <v>39</v>
       </c>
       <c r="B6" s="12" t="s">
-        <v>20</v>
+        <v>33</v>
       </c>
       <c r="C6" s="12" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="D6" s="12" t="s">
-        <v>20</v>
+        <v>35</v>
       </c>
       <c r="E6" s="12" t="s">
-        <v>20</v>
+        <v>34</v>
       </c>
       <c r="F6" s="12" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="G6" s="12" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="H6" s="12" t="s">
-        <v>20</v>
+        <v>36</v>
+      </c>
+      <c r="J6">
+        <v>3</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="12" t="s">
-        <v>20</v>
+        <v>40</v>
       </c>
       <c r="B7" s="12" t="s">
-        <v>20</v>
+        <v>46</v>
       </c>
       <c r="C7" s="12" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="D7" s="12" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="E7" s="12" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="F7" s="12" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="G7" s="12" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="H7" s="12" t="s">
-        <v>20</v>
+        <v>26</v>
+      </c>
+      <c r="I7">
+        <v>10</v>
+      </c>
+      <c r="J7">
+        <v>4</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="12" t="s">
-        <v>20</v>
+        <v>41</v>
       </c>
       <c r="B8" s="12" t="s">
-        <v>20</v>
+        <v>47</v>
       </c>
       <c r="C8" s="12" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="D8" s="12" t="s">
-        <v>20</v>
+        <v>29</v>
       </c>
       <c r="E8" s="12" t="s">
-        <v>20</v>
+        <v>28</v>
       </c>
       <c r="F8" s="12" t="s">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="G8" s="12" t="s">
-        <v>20</v>
+        <v>31</v>
       </c>
       <c r="H8" s="12" t="s">
-        <v>20</v>
+        <v>32</v>
+      </c>
+      <c r="J8">
+        <v>5</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="12" t="s">
-        <v>20</v>
+        <v>42</v>
       </c>
       <c r="B9" s="12" t="s">
-        <v>20</v>
+        <v>48</v>
       </c>
       <c r="C9" s="12" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="D9" s="12" t="s">
-        <v>20</v>
+        <v>35</v>
       </c>
       <c r="E9" s="12" t="s">
-        <v>20</v>
+        <v>34</v>
       </c>
       <c r="F9" s="12" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="G9" s="12" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="H9" s="12" t="s">
-        <v>20</v>
+        <v>36</v>
+      </c>
+      <c r="J9">
+        <v>6</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="12" t="s">
-        <v>20</v>
+        <v>43</v>
       </c>
       <c r="B10" s="12" t="s">
-        <v>20</v>
+        <v>49</v>
       </c>
       <c r="C10" s="12" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="D10" s="12" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="E10" s="12" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="F10" s="12" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="G10" s="12" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="H10" s="12" t="s">
-        <v>20</v>
+        <v>26</v>
+      </c>
+      <c r="I10">
+        <v>10</v>
+      </c>
+      <c r="J10">
+        <v>7</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="12" t="s">
-        <v>20</v>
+        <v>44</v>
       </c>
       <c r="B11" s="12" t="s">
-        <v>20</v>
+        <v>50</v>
       </c>
       <c r="C11" s="12" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="D11" s="12" t="s">
-        <v>20</v>
+        <v>29</v>
       </c>
       <c r="E11" s="12" t="s">
-        <v>20</v>
+        <v>28</v>
       </c>
       <c r="F11" s="12" t="s">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="G11" s="12" t="s">
-        <v>20</v>
+        <v>31</v>
       </c>
       <c r="H11" s="12" t="s">
-        <v>20</v>
+        <v>32</v>
+      </c>
+      <c r="J11">
+        <v>8</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="12" t="s">
-        <v>20</v>
+        <v>45</v>
       </c>
       <c r="B12" s="12" t="s">
-        <v>20</v>
+        <v>51</v>
       </c>
       <c r="C12" s="12" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="D12" s="12" t="s">
-        <v>20</v>
+        <v>35</v>
       </c>
       <c r="E12" s="12" t="s">
-        <v>20</v>
+        <v>34</v>
       </c>
       <c r="F12" s="12" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="G12" s="12" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="H12" s="12" t="s">
-        <v>20</v>
+        <v>36</v>
+      </c>
+      <c r="J12">
+        <v>9</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
@@ -3158,13 +3236,221 @@
         <v>20</v>
       </c>
       <c r="H92" s="12" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="93" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A93" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="B93" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="C93" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="D93" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="E93" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="F93" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="G93" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="H93" s="12" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="94" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A94" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="B94" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="C94" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="D94" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="E94" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="F94" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="G94" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="H94" s="12" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="95" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A95" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="B95" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="C95" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="D95" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="E95" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="F95" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="G95" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="H95" s="12" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="96" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A96" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="B96" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="C96" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="D96" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="E96" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="F96" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="G96" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="H96" s="12" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="97" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A97" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="B97" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="C97" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="D97" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="E97" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="F97" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="G97" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="H97" s="12" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="98" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A98" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="B98" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="C98" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="D98" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="E98" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="F98" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="G98" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="H98" s="12" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="99" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A99" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="B99" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="C99" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="D99" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="E99" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="F99" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="G99" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="H99" s="12" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="100" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A100" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="B100" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="C100" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="D100" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="E100" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="F100" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="G100" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="H100" s="12" t="s">
         <v>20</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="12" type="noConversion"/>
   <dataValidations count="1">
-    <dataValidation type="whole" operator="greaterThanOrEqual" allowBlank="1" showErrorMessage="1" errorTitle="Lỗi nhập liệu" error="Chỉ được nhập số nguyên lớn hơn hoặc bằng 0!" sqref="I4:J92" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="whole" operator="greaterThanOrEqual" allowBlank="1" showErrorMessage="1" errorTitle="Lỗi nhập liệu" error="Chỉ được nhập số nguyên lớn hơn hoặc bằng 0!" sqref="I4:J100" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>0</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
[update]: cập nhật lại giải pháp phase 3
</commit_message>
<xml_diff>
--- a/assets/files/bm_mailing_danh_gia.xlsx
+++ b/assets/files/bm_mailing_danh_gia.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tuank\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tuank\Revotech\VCC\cbms\test\assets\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47D3EE02-6121-4883-9C63-C3FEBCD42183}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75427530-C0AE-473B-A244-E8533E65FC40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-5475" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="180" windowWidth="28770" windowHeight="15345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Input" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="792" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="792" uniqueCount="45">
   <si>
     <r>
       <t>Mã nhà thầu</t>
@@ -208,6 +208,33 @@
   </si>
   <si>
     <t>400.000</t>
+  </si>
+  <si>
+    <t>NT004</t>
+  </si>
+  <si>
+    <t>Nhà thầu 4</t>
+  </si>
+  <si>
+    <t>8.000.000</t>
+  </si>
+  <si>
+    <t>NT005</t>
+  </si>
+  <si>
+    <t>Nhà thầu 5</t>
+  </si>
+  <si>
+    <t>NT006</t>
+  </si>
+  <si>
+    <t>Nhà thầu 6</t>
+  </si>
+  <si>
+    <t>9.000.000</t>
+  </si>
+  <si>
+    <t>10.000.000</t>
   </si>
 </sst>
 </file>
@@ -686,7 +713,7 @@
   <dimension ref="A1:H100"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -825,7 +852,7 @@
         <v>26</v>
       </c>
       <c r="G5" s="10" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H5" s="10" t="s">
         <v>28</v>
@@ -859,80 +886,80 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="10" t="s">
-        <v>16</v>
+        <v>36</v>
       </c>
       <c r="B7" s="10" t="s">
-        <v>16</v>
+        <v>37</v>
       </c>
       <c r="C7" s="10" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="D7" s="10" t="s">
-        <v>16</v>
+        <v>38</v>
       </c>
       <c r="E7" s="10" t="s">
-        <v>16</v>
+        <v>33</v>
       </c>
       <c r="F7" s="10" t="s">
-        <v>16</v>
+        <v>34</v>
       </c>
       <c r="G7" s="10" t="s">
-        <v>16</v>
+        <v>27</v>
       </c>
       <c r="H7" s="10" t="s">
-        <v>16</v>
+        <v>35</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="10" t="s">
-        <v>16</v>
+        <v>39</v>
       </c>
       <c r="B8" s="10" t="s">
-        <v>16</v>
+        <v>40</v>
       </c>
       <c r="C8" s="10" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="D8" s="10" t="s">
-        <v>16</v>
+        <v>43</v>
       </c>
       <c r="E8" s="10" t="s">
-        <v>16</v>
+        <v>33</v>
       </c>
       <c r="F8" s="10" t="s">
-        <v>16</v>
+        <v>34</v>
       </c>
       <c r="G8" s="10" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="H8" s="10" t="s">
-        <v>16</v>
+        <v>35</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="10" t="s">
-        <v>16</v>
+        <v>41</v>
       </c>
       <c r="B9" s="10" t="s">
-        <v>16</v>
+        <v>42</v>
       </c>
       <c r="C9" s="10" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="D9" s="10" t="s">
-        <v>16</v>
+        <v>44</v>
       </c>
       <c r="E9" s="10" t="s">
-        <v>16</v>
+        <v>33</v>
       </c>
       <c r="F9" s="10" t="s">
-        <v>16</v>
+        <v>34</v>
       </c>
       <c r="G9" s="10" t="s">
-        <v>16</v>
+        <v>25</v>
       </c>
       <c r="H9" s="10" t="s">
-        <v>16</v>
+        <v>35</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">

</xml_diff>